<commit_message>
added code for inserting final scores
</commit_message>
<xml_diff>
--- a/AUT.xlsx
+++ b/AUT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8596" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8596" uniqueCount="1323">
   <si>
     <t>A..Klagenfurt</t>
   </si>
@@ -3975,9 +3975,6 @@
   </si>
   <si>
     <t>33.8%</t>
-  </si>
-  <si>
-    <t>40.0%</t>
   </si>
   <si>
     <t>N</t>
@@ -49394,13 +49391,13 @@
         <v>1311</v>
       </c>
       <c r="C11" t="s">
-        <v>1178</v>
+        <v>939</v>
       </c>
       <c r="D11" t="s">
-        <v>923</v>
+        <v>1098</v>
       </c>
       <c r="E11" t="s">
-        <v>1317</v>
+        <v>1084</v>
       </c>
     </row>
   </sheetData>
@@ -49422,10 +49419,10 @@
         <v>1300</v>
       </c>
       <c r="C1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D1" t="s">
         <v>1318</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1319</v>
       </c>
     </row>
     <row r="2">
@@ -49439,7 +49436,7 @@
         <v>813</v>
       </c>
       <c r="D2" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="3">
@@ -49450,7 +49447,7 @@
         <v>1303</v>
       </c>
       <c r="C3" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="D3" t="s">
         <v>1050</v>
@@ -49509,7 +49506,7 @@
         <v>771</v>
       </c>
       <c r="D7" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="8">
@@ -49537,7 +49534,7 @@
         <v>1046</v>
       </c>
       <c r="D9" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="10">
@@ -49562,10 +49559,10 @@
         <v>1311</v>
       </c>
       <c r="C11" t="s">
-        <v>904</v>
+        <v>922</v>
       </c>
       <c r="D11" t="s">
-        <v>1035</v>
+        <v>1275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated divisions to last 6
</commit_message>
<xml_diff>
--- a/AUT.xlsx
+++ b/AUT.xlsx
@@ -401,256 +401,256 @@
     <t>Team against</t>
   </si>
   <si>
-    <t>A. Klagenfurt,D L W D L W L D W D D</t>
-  </si>
-  <si>
-    <t>Admira,D W L L L D W D L W D</t>
-  </si>
-  <si>
-    <t>Altach,L W L W D L D D L L D</t>
-  </si>
-  <si>
-    <t>Austria Vienna,L D L D D D W D W L D</t>
-  </si>
-  <si>
-    <t>Hartberg,W L L D D L W D L W D</t>
-  </si>
-  <si>
-    <t>LASK,W D D L D L L D W L L</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,L D W L W D L L L W D</t>
-  </si>
-  <si>
-    <t>Ried,W L W D L W D D L D L</t>
-  </si>
-  <si>
-    <t>Salzburg,W W W W W W W W W W D</t>
-  </si>
-  <si>
-    <t>Sturm Graz,L W W W D D W W W L W</t>
-  </si>
-  <si>
-    <t>Tirol,D D D D D L L L W L D</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,D L L D W W L D L W W</t>
-  </si>
-  <si>
-    <t>A. Klagenfurt,1 0 4 1 1 2 1 1 4 1 1,(17)</t>
-  </si>
-  <si>
-    <t>Admira,1 4 1 0 0 1 2 1 1 2 2,(15)</t>
-  </si>
-  <si>
-    <t>Altach,0 2 1 2 0 1 1 0 0 0 1,(8)</t>
-  </si>
-  <si>
-    <t>Austria Vienna,1 1 0 1 2 1 2 0 4 0 2,(14)</t>
-  </si>
-  <si>
-    <t>Hartberg,2 1 3 1 1 0 3 1 3 3 2,(20)</t>
-  </si>
-  <si>
-    <t>LASK,1 1 1 1 1 0 0 1 3 1 0,(10)</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,0 1 3 1 3 1 1 0 0 5 1,(16)</t>
-  </si>
-  <si>
-    <t>Ried,2 1 2 1 0 1 1 3 2 1 0,(14)</t>
-  </si>
-  <si>
-    <t>Salzburg,3 7 1 1 3 1 3 2 2 3 1,(27)</t>
-  </si>
-  <si>
-    <t>Sturm Graz,1 4 3 3 2 1 2 5 3 2 1,(27)</t>
-  </si>
-  <si>
-    <t>Tirol,1 1 1 2 0 1 1 0 4 2 2,(15)</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,1 1 0 2 3 2 1 3 0 1 1,(15)</t>
-  </si>
-  <si>
-    <t>A. Klagenfurt,1 4 3 1 3 1 2 1 0 1 1,(18)</t>
-  </si>
-  <si>
-    <t>Admira,1 0 2 1 3 1 1 1 3 0 2,(15)</t>
-  </si>
-  <si>
-    <t>Altach,1 1 3 1 0 2 1 0 4 2 1,(16)</t>
-  </si>
-  <si>
-    <t>Austria Vienna,2 1 1 1 2 1 0 0 3 1 2,(14)</t>
-  </si>
-  <si>
-    <t>Hartberg,0 2 4 1 1 1 1 1 4 2 2,(19)</t>
-  </si>
-  <si>
-    <t>LASK,0 1 1 3 1 1 2 1 1 3 1,(15)</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,2 1 0 2 0 1 2 2 3 2 1,(16)</t>
-  </si>
-  <si>
-    <t>Ried,1 7 1 1 3 0 1 3 4 1 1,(23)</t>
-  </si>
-  <si>
-    <t>Salzburg,1 1 0 0 1 0 1 0 0 1 1,(6)</t>
-  </si>
-  <si>
-    <t>Sturm Graz,3 1 1 1 2 1 1 0 0 3 0,(13)</t>
-  </si>
-  <si>
-    <t>Tirol,1 1 1 2 0 2 3 5 2 5 2,(24)</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,1 4 3 2 0 1 3 3 2 0 0,(19)</t>
-  </si>
-  <si>
-    <t>A. Klagenfurt,2 4 7 2 4 3 3 2 4 2 2,(35)</t>
-  </si>
-  <si>
-    <t>Admira,2 4 3 1 3 2 3 2 4 2 4,(30)</t>
-  </si>
-  <si>
-    <t>Altach,1 3 4 3 0 3 2 0 4 2 2,(24)</t>
-  </si>
-  <si>
-    <t>Austria Vienna,3 2 1 2 4 2 2 0 7 1 4,(28)</t>
-  </si>
-  <si>
-    <t>Hartberg,2 3 7 2 2 1 4 2 7 5 4,(39)</t>
-  </si>
-  <si>
-    <t>LASK,1 2 2 4 2 1 2 2 4 4 1,(25)</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,2 2 3 3 3 2 3 2 3 7 2,(32)</t>
-  </si>
-  <si>
-    <t>Ried,3 8 3 2 3 1 2 6 6 2 1,(37)</t>
-  </si>
-  <si>
-    <t>Salzburg,4 8 1 1 4 1 4 2 2 4 2,(33)</t>
-  </si>
-  <si>
-    <t>Sturm Graz,4 5 4 4 4 2 3 5 3 5 1,(40)</t>
-  </si>
-  <si>
-    <t>Tirol,2 2 2 4 0 3 4 5 6 7 4,(39)</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,2 5 3 4 3 3 4 6 2 1 1,(34)</t>
-  </si>
-  <si>
-    <t>A. Klagenfurt,1-1 4-0 4-3 1-1 3-1 2-1 2-1 1-1 0-4 1-1 1-1</t>
-  </si>
-  <si>
-    <t>Admira,1-1 4-0 2-1 0-1 3-0 1-1 1-2 1-1 3-1 2-0 2-2</t>
-  </si>
-  <si>
-    <t>Altach,0-1 1-2 3-1 2-1 0-0 1-2 1-1 0-0 0-4 2-0 1-1</t>
-  </si>
-  <si>
-    <t>Austria Vienna,2-1 1-1 1-0 1-1 2-2 1-1 0-2 0-0 3-4 1-0 2-2</t>
-  </si>
-  <si>
-    <t>Hartberg,0-2 1-2 4-3 1-1 1-1 0-1 1-3 1-1 3-4 3-2 2-2</t>
-  </si>
-  <si>
-    <t>LASK,0-1 1-1 1-1 1-3 1-1 1-0 0-2 1-1 3-1 3-1 0-1</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,0-2 1-1 3-0 2-1 3-0 1-1 1-2 2-0 0-3 5-2 1-1</t>
-  </si>
-  <si>
-    <t>Ried,2-1 7-1 2-1 1-1 3-0 1-0 1-1 3-3 4-2 1-1 1-0</t>
-  </si>
-  <si>
-    <t>Salzburg,1-3 7-1 1-0 0-1 3-1 0-1 1-3 2-0 0-2 3-1 1-1</t>
-  </si>
-  <si>
-    <t>Sturm Graz,1-3 1-4 3-1 1-3 2-2 1-1 2-1 5-0 0-3 3-2 1-0</t>
-  </si>
-  <si>
-    <t>Tirol,1-1 1-1 1-1 2-2 0-0 2-1 1-3 5-0 4-2 5-2 2-2</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,1-1 1-4 3-0 2-2 3-0 1-2 1-3 3-3 0-2 1-0 0-1</t>
-  </si>
-  <si>
-    <t>A. Klagenfurt,0 -4 1 0 -2 1 -1 0 4 0 0,(-1)</t>
-  </si>
-  <si>
-    <t>Admira,0 4 -1 -1 -3 0 1 0 -2 2 0,(0)</t>
-  </si>
-  <si>
-    <t>Altach,-1 1 -2 1 0 -1 0 0 -4 -2 0,(-8)</t>
-  </si>
-  <si>
-    <t>Austria Vienna,-1 0 -1 0 0 0 2 0 1 -1 0,(0)</t>
-  </si>
-  <si>
-    <t>Hartberg,2 -1 -1 0 0 -1 2 0 -1 1 0,(1)</t>
-  </si>
-  <si>
-    <t>LASK,1 0 0 -2 0 -1 -2 0 2 -2 -1,(-5)</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,-2 0 3 -1 3 0 -1 -2 -3 3 0,(0)</t>
-  </si>
-  <si>
-    <t>Ried,1 -6 1 0 -3 1 0 0 -2 0 -1,(-9)</t>
-  </si>
-  <si>
-    <t>Salzburg,2 6 1 1 2 1 2 2 2 2 0,(21)</t>
-  </si>
-  <si>
-    <t>Sturm Graz,-2 3 2 2 0 0 1 5 3 -1 1,(14)</t>
-  </si>
-  <si>
-    <t>Tirol,0 0 0 0 0 -1 -2 -5 2 -3 0,(-9)</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,0 -3 -3 0 3 1 -2 0 -2 1 1,(-4)</t>
-  </si>
-  <si>
-    <t>A. Klagenfurt,Wolfsberger AC(3) Admira(5) Hartberg(6) Austria Vienna(8) Salzburg(1) Tirol(12) Sturm Graz(2) LASK(11) Altach(10) Ried(7) Rapid Vienna(9)</t>
-  </si>
-  <si>
-    <t>Admira,Tirol(12) A. Klagenfurt(4) Ried(7) Salzburg(1) Wolfsberger AC(3) Sturm Graz(2) Rapid Vienna(9) Hartberg(6) LASK(11) Altach(10) Austria Vienna(8)</t>
-  </si>
-  <si>
-    <t>Altach,LASK(11) Hartberg(6) Sturm Graz(2) Rapid Vienna(9) Tirol(12) Wolfsberger AC(3) Ried(7) Austria Vienna(8) A. Klagenfurt(4) Admira(5) Salzburg(1)</t>
-  </si>
-  <si>
-    <t>Austria Vienna,Ried(7) Tirol(12) Salzburg(1) A. Klagenfurt(4) Sturm Graz(2) Rapid Vienna(9) LASK(11) Altach(10) Hartberg(6) Wolfsberger AC(3) Admira(5)</t>
-  </si>
-  <si>
-    <t>Hartberg,Rapid Vienna(9) Altach(10) A. Klagenfurt(4) Ried(7) LASK(11) Salzburg(1) Wolfsberger AC(3) Admira(5) Austria Vienna(8) Sturm Graz(2) Tirol(12)</t>
-  </si>
-  <si>
-    <t>LASK,Altach(10) Rapid Vienna(9) Tirol(12) Sturm Graz(2) Hartberg(6) Ried(7) Austria Vienna(8) A. Klagenfurt(4) Admira(5) Salzburg(1) Wolfsberger AC(3)</t>
-  </si>
-  <si>
-    <t>Rapid Vienna,Hartberg(6) LASK(11) Wolfsberger AC(3) Altach(10) Ried(7) Austria Vienna(8) Admira(5) Salzburg(1) Sturm Graz(2) Tirol(12) A. Klagenfurt(4)</t>
-  </si>
-  <si>
-    <t>Ried,Austria Vienna(8) Salzburg(1) Admira(5) Hartberg(6) Rapid Vienna(9) LASK(11) Altach(10) Wolfsberger AC(3) Tirol(12) A. Klagenfurt(4) Sturm Graz(2)</t>
-  </si>
-  <si>
-    <t>Salzburg,Sturm Graz(2) Ried(7) Austria Vienna(8) Admira(5) A. Klagenfurt(4) Hartberg(6) Tirol(12) Rapid Vienna(9) Wolfsberger AC(3) LASK(11) Altach(10)</t>
-  </si>
-  <si>
-    <t>Sturm Graz,Salzburg(1) Wolfsberger AC(3) Altach(10) LASK(11) Austria Vienna(8) Admira(5) A. Klagenfurt(4) Tirol(12) Rapid Vienna(9) Hartberg(6) Ried(7)</t>
-  </si>
-  <si>
-    <t>Tirol,Admira(5) Austria Vienna(8) LASK(11) Wolfsberger AC(3) Altach(10) A. Klagenfurt(4) Salzburg(1) Sturm Graz(2) Ried(7) Rapid Vienna(9) Hartberg(6)</t>
-  </si>
-  <si>
-    <t>Wolfsberger AC,A. Klagenfurt(4) Sturm Graz(2) Rapid Vienna(9) Tirol(12) Admira(5) Altach(10) Hartberg(6) Ried(7) Salzburg(1) Austria Vienna(8) LASK(11)</t>
+    <t>A. Klagenfurt,W L D W D D</t>
+  </si>
+  <si>
+    <t>Admira,D W D L W D</t>
+  </si>
+  <si>
+    <t>Altach,L D D L L D</t>
+  </si>
+  <si>
+    <t>Austria Vienna,D W D W L D</t>
+  </si>
+  <si>
+    <t>Hartberg,L W D L W D</t>
+  </si>
+  <si>
+    <t>LASK,L L D W L L</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,D L L L W D</t>
+  </si>
+  <si>
+    <t>Ried,W D D L D L</t>
+  </si>
+  <si>
+    <t>Salzburg,W W W W W D</t>
+  </si>
+  <si>
+    <t>Sturm Graz,D W W W L W</t>
+  </si>
+  <si>
+    <t>Tirol,L L L W L D</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,W L D L W W</t>
+  </si>
+  <si>
+    <t>A. Klagenfurt,2 1 1 4 1 1,(10)</t>
+  </si>
+  <si>
+    <t>Admira,1 2 1 1 2 2,(9)</t>
+  </si>
+  <si>
+    <t>Altach,1 1 0 0 0 1,(3)</t>
+  </si>
+  <si>
+    <t>Austria Vienna,1 2 0 4 0 2,(9)</t>
+  </si>
+  <si>
+    <t>Hartberg,0 3 1 3 3 2,(12)</t>
+  </si>
+  <si>
+    <t>LASK,0 0 1 3 1 0,(5)</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,1 1 0 0 5 1,(8)</t>
+  </si>
+  <si>
+    <t>Ried,1 1 3 2 1 0,(8)</t>
+  </si>
+  <si>
+    <t>Salzburg,1 3 2 2 3 1,(12)</t>
+  </si>
+  <si>
+    <t>Sturm Graz,1 2 5 3 2 1,(14)</t>
+  </si>
+  <si>
+    <t>Tirol,1 1 0 4 2 2,(10)</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,2 1 3 0 1 1,(8)</t>
+  </si>
+  <si>
+    <t>A. Klagenfurt,1 2 1 0 1 1,(6)</t>
+  </si>
+  <si>
+    <t>Admira,1 1 1 3 0 2,(8)</t>
+  </si>
+  <si>
+    <t>Altach,2 1 0 4 2 1,(10)</t>
+  </si>
+  <si>
+    <t>Austria Vienna,1 0 0 3 1 2,(7)</t>
+  </si>
+  <si>
+    <t>Hartberg,1 1 1 4 2 2,(11)</t>
+  </si>
+  <si>
+    <t>LASK,1 2 1 1 3 1,(9)</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,1 2 2 3 2 1,(11)</t>
+  </si>
+  <si>
+    <t>Ried,0 1 3 4 1 1,(10)</t>
+  </si>
+  <si>
+    <t>Salzburg,0 1 0 0 1 1,(3)</t>
+  </si>
+  <si>
+    <t>Sturm Graz,1 1 0 0 3 0,(5)</t>
+  </si>
+  <si>
+    <t>Tirol,2 3 5 2 5 2,(19)</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,1 3 3 2 0 0,(9)</t>
+  </si>
+  <si>
+    <t>A. Klagenfurt,3 3 2 4 2 2,(16)</t>
+  </si>
+  <si>
+    <t>Admira,2 3 2 4 2 4,(17)</t>
+  </si>
+  <si>
+    <t>Altach,3 2 0 4 2 2,(13)</t>
+  </si>
+  <si>
+    <t>Austria Vienna,2 2 0 7 1 4,(16)</t>
+  </si>
+  <si>
+    <t>Hartberg,1 4 2 7 5 4,(23)</t>
+  </si>
+  <si>
+    <t>LASK,1 2 2 4 4 1,(14)</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,2 3 2 3 7 2,(19)</t>
+  </si>
+  <si>
+    <t>Ried,1 2 6 6 2 1,(18)</t>
+  </si>
+  <si>
+    <t>Salzburg,1 4 2 2 4 2,(15)</t>
+  </si>
+  <si>
+    <t>Sturm Graz,2 3 5 3 5 1,(19)</t>
+  </si>
+  <si>
+    <t>Tirol,3 4 5 6 7 4,(29)</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,3 4 6 2 1 1,(17)</t>
+  </si>
+  <si>
+    <t>A. Klagenfurt,2-1 2-1 1-1 0-4 1-1 1-1</t>
+  </si>
+  <si>
+    <t>Admira,1-1 1-2 1-1 3-1 2-0 2-2</t>
+  </si>
+  <si>
+    <t>Altach,1-2 1-1 0-0 0-4 2-0 1-1</t>
+  </si>
+  <si>
+    <t>Austria Vienna,1-1 0-2 0-0 3-4 1-0 2-2</t>
+  </si>
+  <si>
+    <t>Hartberg,0-1 1-3 1-1 3-4 3-2 2-2</t>
+  </si>
+  <si>
+    <t>LASK,1-0 0-2 1-1 3-1 3-1 0-1</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,1-1 1-2 2-0 0-3 5-2 1-1</t>
+  </si>
+  <si>
+    <t>Ried,1-0 1-1 3-3 4-2 1-1 1-0</t>
+  </si>
+  <si>
+    <t>Salzburg,0-1 1-3 2-0 0-2 3-1 1-1</t>
+  </si>
+  <si>
+    <t>Sturm Graz,1-1 2-1 5-0 0-3 3-2 1-0</t>
+  </si>
+  <si>
+    <t>Tirol,2-1 1-3 5-0 4-2 5-2 2-2</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,1-2 1-3 3-3 0-2 1-0 0-1</t>
+  </si>
+  <si>
+    <t>A. Klagenfurt,1 -1 0 4 0 0,(4)</t>
+  </si>
+  <si>
+    <t>Admira,0 1 0 -2 2 0,(1)</t>
+  </si>
+  <si>
+    <t>Altach,-1 0 0 -4 -2 0,(-7)</t>
+  </si>
+  <si>
+    <t>Austria Vienna,0 2 0 1 -1 0,(2)</t>
+  </si>
+  <si>
+    <t>Hartberg,-1 2 0 -1 1 0,(1)</t>
+  </si>
+  <si>
+    <t>LASK,-1 -2 0 2 -2 -1,(-4)</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,0 -1 -2 -3 3 0,(-3)</t>
+  </si>
+  <si>
+    <t>Ried,1 0 0 -2 0 -1,(-2)</t>
+  </si>
+  <si>
+    <t>Salzburg,1 2 2 2 2 0,(9)</t>
+  </si>
+  <si>
+    <t>Sturm Graz,0 1 5 3 -1 1,(9)</t>
+  </si>
+  <si>
+    <t>Tirol,-1 -2 -5 2 -3 0,(-9)</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,1 -2 0 -2 1 1,(-1)</t>
+  </si>
+  <si>
+    <t>A. Klagenfurt,Tirol(12) Sturm Graz(2) LASK(11) Altach(10) Ried(7) Rapid Vienna(9)</t>
+  </si>
+  <si>
+    <t>Admira,Sturm Graz(2) Rapid Vienna(9) Hartberg(6) LASK(11) Altach(10) Austria Vienna(8)</t>
+  </si>
+  <si>
+    <t>Altach,Wolfsberger AC(3) Ried(7) Austria Vienna(8) A. Klagenfurt(4) Admira(5) Salzburg(1)</t>
+  </si>
+  <si>
+    <t>Austria Vienna,Rapid Vienna(9) LASK(11) Altach(10) Hartberg(6) Wolfsberger AC(3) Admira(5)</t>
+  </si>
+  <si>
+    <t>Hartberg,Salzburg(1) Wolfsberger AC(3) Admira(5) Austria Vienna(8) Sturm Graz(2) Tirol(12)</t>
+  </si>
+  <si>
+    <t>LASK,Ried(7) Austria Vienna(8) A. Klagenfurt(4) Admira(5) Salzburg(1) Wolfsberger AC(3)</t>
+  </si>
+  <si>
+    <t>Rapid Vienna,Austria Vienna(8) Admira(5) Salzburg(1) Sturm Graz(2) Tirol(12) A. Klagenfurt(4)</t>
+  </si>
+  <si>
+    <t>Ried,LASK(11) Altach(10) Wolfsberger AC(3) Tirol(12) A. Klagenfurt(4) Sturm Graz(2)</t>
+  </si>
+  <si>
+    <t>Salzburg,Hartberg(6) Tirol(12) Rapid Vienna(9) Wolfsberger AC(3) LASK(11) Altach(10)</t>
+  </si>
+  <si>
+    <t>Sturm Graz,Admira(5) A. Klagenfurt(4) Tirol(12) Rapid Vienna(9) Hartberg(6) Ried(7)</t>
+  </si>
+  <si>
+    <t>Tirol,A. Klagenfurt(4) Salzburg(1) Sturm Graz(2) Ried(7) Rapid Vienna(9) Hartberg(6)</t>
+  </si>
+  <si>
+    <t>Wolfsberger AC,Altach(10) Hartberg(6) Ried(7) Salzburg(1) Austria Vienna(8) LASK(11)</t>
   </si>
   <si>
     <t>aut_division</t>

</xml_diff>